<commit_message>
Added scalable heuristic strategy
</commit_message>
<xml_diff>
--- a/Data/promocje_księgarnie.xlsx
+++ b/Data/promocje_księgarnie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariannakolinko/Desktop/NOTATKI/MAGISTERKA/ROK II/SEM LETNI S2-2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xbots\OneDrive\Pulpit\Project books\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD7AE3AF-B6C9-374B-BC9A-C90AC8002538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03FBD25-AFEF-4C03-8EBD-1D9558796AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1000" windowWidth="27840" windowHeight="15260" xr2:uid="{3995E3DB-F2A4-CF48-8B1C-220A01B8C9BF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3995E3DB-F2A4-CF48-8B1C-220A01B8C9BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -62,20 +62,20 @@
     <t>1+1 gratis</t>
   </si>
   <si>
-    <t>total_price -= sum(prices[:len(prices)//2])</t>
-  </si>
-  <si>
     <t>Rabat -10% od 3 sztuk</t>
   </si>
   <si>
     <t>if len(prices) &gt;= 3: total_price *= 0.9</t>
+  </si>
+  <si>
+    <t>if len(prices) &gt;= 2: total_price -= sorted(prices)[1] * 0.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -91,6 +91,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -111,15 +117,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny 2" xfId="1" xr:uid="{D488B8AA-C15D-4C0D-9364-B1FAE2AB2B57}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -454,17 +462,17 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
-    <col min="3" max="3" width="36.83203125" customWidth="1"/>
+    <col min="1" max="1" width="22.69921875" customWidth="1"/>
+    <col min="2" max="2" width="27.69921875" customWidth="1"/>
+    <col min="3" max="3" width="36.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +483,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -486,12 +494,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -502,18 +510,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -521,7 +529,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>